<commit_message>
:sparkles: Extracted some cell codes
</commit_message>
<xml_diff>
--- a/sample/copy-sheet/output.xlsx
+++ b/sample/copy-sheet/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="6">
   <si>
     <t>联系方式</t>
   </si>
@@ -126,12 +126,19 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>多</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
         <color theme="5"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>种</t>
@@ -140,9 +147,96 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>多</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>种</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>多</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>种</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="28"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
     </r>
   </si>
   <si>
@@ -159,7 +253,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="157">
+  <fonts count="164">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -363,6 +457,13 @@
     </font>
     <font>
       <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
       <sz val="11.0"/>
       <u val="none"/>
       <color indexed="0"/>
@@ -374,6 +475,22 @@
       <u val="none"/>
       <color indexed="0"/>
       <charset val="0"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <name val="宋体"/>
@@ -391,27 +508,26 @@
     </font>
     <font>
       <name val="宋体"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <name val="宋体"/>
       <sz val="11.0"/>
       <b val="true"/>
       <u val="none"/>
       <color indexed="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <i val="true"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="18.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="134"/>
+      <charset val="0"/>
     </font>
     <font>
       <name val="宋体"/>
@@ -424,55 +540,9 @@
     <font>
       <name val="宋体"/>
       <sz val="11.0"/>
-      <b val="true"/>
       <u val="none"/>
       <color indexed="0"/>
       <charset val="0"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <sz val="13.0"/>
-      <b val="true"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="134"/>
     </font>
     <font>
       <name val="宋体"/>
@@ -490,13 +560,6 @@
     </font>
     <font>
       <name val="宋体"/>
-      <sz val="11.0"/>
-      <u val="none"/>
-      <color indexed="0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="宋体"/>
       <sz val="15.0"/>
       <b val="true"/>
       <u val="none"/>
@@ -505,7 +568,60 @@
     </font>
     <font>
       <name val="宋体"/>
-      <sz val="12.0"/>
+      <sz val="13.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <u val="none"/>
+      <color indexed="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="28.0"/>
       <u val="none"/>
       <color indexed="0"/>
       <charset val="134"/>
@@ -1066,10 +1182,9 @@
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
-      <main:color theme="1" rgb="000000"/>
-      <main:name val="宋体"/>
-      <main:charset val="134"/>
-      <main:scheme val="minor"/>
+      <main:color theme="1"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
     </font>
     <font>
       <name val="宋体"/>
@@ -1120,6 +1235,22 @@
       <color rgb="000000"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:i/>
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <i val="true"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <main:sz val="12"/>
       <main:color theme="1" rgb="000000"/>
       <main:name val="宋体"/>
@@ -1165,6 +1296,19 @@
       <main:color theme="1" rgb="000000"/>
       <main:name val="宋体"/>
       <main:charset val="134"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <sz val="12.0"/>
+      <u val="none"/>
+      <charset val="134"/>
+      <color rgb="000000"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:sz val="12"/>
+      <main:color theme="1" rgb="000000"/>
+      <main:name val="宋体"/>
+      <main:charset val="134"/>
       <main:scheme val="minor"/>
     </font>
     <font>
@@ -1271,7 +1415,7 @@
       <color rgb="000000"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1463,6 +1607,18 @@
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
+    </fill>
+    <fill xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:patternFill patternType="solid">
+        <main:fgColor theme="7" tint="0.8" rgb="FFC000"/>
+        <main:bgColor indexed="64"/>
+      </main:patternFill>
+    </fill>
+    <fill xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:patternFill patternType="solid">
+        <main:fgColor theme="9" tint="0.8" rgb="70AD47"/>
+        <main:bgColor indexed="64"/>
+      </main:patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -1721,7 +1877,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1737,169 +1893,175 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="106" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="109" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="108" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="114" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="121" fillId="33" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="1" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="135" fillId="34" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="1" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="141" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="143" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="142" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="144" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="147" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyNumberFormat="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="146" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="148" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="153" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="157" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="154" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
-      <main:alignment vertical="center"/>
-    </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="159" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="161" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment vertical="center"/>
+    </xf>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="163" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2586,7 +2748,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" ht="17.6" customHeight="true">
+    <row r="14" ht="18.0" customHeight="true">
       <c r="A14" t="n" s="46">
         <v>12.0</v>
       </c>
@@ -2596,45 +2758,51 @@
       <c r="C14" t="n" s="48">
         <v>33.0</v>
       </c>
-    </row>
-    <row r="15" ht="17.6" customHeight="true">
-      <c r="A15" t="n" s="49">
+      <c r="G14" t="s" s="49">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" ht="40.0" customHeight="true">
+      <c r="A15" t="n" s="50">
         <v>13.0</v>
       </c>
-      <c r="B15" t="s" s="50">
+      <c r="B15" t="s" s="51">
         <v>28</v>
       </c>
-      <c r="C15" t="n" s="51">
+      <c r="C15" t="n" s="52">
         <v>27.0</v>
       </c>
+      <c r="G15" t="s" s="53">
+        <v>38</v>
+      </c>
     </row>
     <row r="16" ht="17.6" customHeight="true">
-      <c r="A16" t="n" s="52">
+      <c r="A16" t="n" s="54">
         <v>14.0</v>
       </c>
-      <c r="B16" t="s" s="53">
+      <c r="B16" t="s" s="55">
         <v>30</v>
       </c>
-      <c r="C16" t="n" s="54">
+      <c r="C16" t="n" s="56">
         <v>20.0</v>
       </c>
     </row>
     <row r="17" ht="17.6" customHeight="true">
-      <c r="A17" t="n" s="55">
+      <c r="A17" t="n" s="57">
         <v>15.0</v>
       </c>
-      <c r="B17" t="s" s="56">
+      <c r="B17" t="s" s="58">
         <v>32</v>
       </c>
-      <c r="C17" t="n" s="57">
+      <c r="C17" t="n" s="59">
         <v>28.0</v>
       </c>
     </row>
     <row r="18" ht="17.6" customHeight="true">
-      <c r="B18" t="s" s="58">
-        <v>37</v>
-      </c>
-      <c r="C18" s="59" t="n">
+      <c r="B18" t="s" s="60">
+        <v>39</v>
+      </c>
+      <c r="C18" s="61" t="n">
         <f>SUM(C3:C17)</f>
         <v>414.0</v>
       </c>

</xml_diff>